<commit_message>
Some more timing result changes
</commit_message>
<xml_diff>
--- a/report/timing.xlsx
+++ b/report/timing.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t xml:space="preserve">Function: </t>
   </si>
@@ -610,11 +610,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="245023504"/>
-        <c:axId val="245020760"/>
+        <c:axId val="309756944"/>
+        <c:axId val="309757728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="245023504"/>
+        <c:axId val="309756944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,12 +726,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245020760"/>
+        <c:crossAx val="309757728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245020760"/>
+        <c:axId val="309757728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245023504"/>
+        <c:crossAx val="309756944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1408,11 +1408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="245024680"/>
-        <c:axId val="245027032"/>
+        <c:axId val="310979096"/>
+        <c:axId val="310977528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="245024680"/>
+        <c:axId val="310979096"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1525,12 +1525,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245027032"/>
+        <c:crossAx val="310977528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245027032"/>
+        <c:axId val="310977528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1642,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245024680"/>
+        <c:crossAx val="310979096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3170,8 +3170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4127,6 +4127,9 @@
       <c r="C63" t="s">
         <v>6</v>
       </c>
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -4136,11 +4139,15 @@
         <v>4.2163100000000003E-7</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" ref="C64:C82" si="6">B64/A64</f>
+        <f t="shared" ref="C64:C77" si="6">B64/A64</f>
         <v>2.1081550000000001E-7</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="1">
+        <f>C64/A64</f>
+        <v>1.0540775000000001E-7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4</v>
       </c>
@@ -4151,8 +4158,12 @@
         <f t="shared" si="6"/>
         <v>1.7803950000000001E-7</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="1">
+        <f t="shared" ref="D65:D77" si="7">C65/A65</f>
+        <v>4.4509875000000003E-8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>8</v>
       </c>
@@ -4163,8 +4174,12 @@
         <f t="shared" si="6"/>
         <v>1.6864000000000001E-7</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="1">
+        <f t="shared" si="7"/>
+        <v>2.1080000000000001E-8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>16</v>
       </c>
@@ -4175,8 +4190,12 @@
         <f t="shared" si="6"/>
         <v>1.8420437500000001E-7</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" s="1">
+        <f t="shared" si="7"/>
+        <v>1.1512773437500001E-8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>32</v>
       </c>
@@ -4187,8 +4206,12 @@
         <f t="shared" si="6"/>
         <v>2.1606437500000001E-7</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" s="1">
+        <f t="shared" si="7"/>
+        <v>6.7520117187500002E-9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>64</v>
       </c>
@@ -4199,8 +4222,12 @@
         <f t="shared" si="6"/>
         <v>2.94525E-7</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" s="1">
+        <f t="shared" si="7"/>
+        <v>4.601953125E-9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>128</v>
       </c>
@@ -4211,8 +4238,12 @@
         <f t="shared" si="6"/>
         <v>4.5901484375E-7</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" s="1">
+        <f t="shared" si="7"/>
+        <v>3.586053466796875E-9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>256</v>
       </c>
@@ -4223,8 +4254,12 @@
         <f t="shared" si="6"/>
         <v>9.8541406250000005E-7</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71" s="1">
+        <f t="shared" si="7"/>
+        <v>3.8492736816406252E-9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>512</v>
       </c>
@@ -4235,8 +4270,12 @@
         <f t="shared" si="6"/>
         <v>2.4788281250000002E-6</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72" s="1">
+        <f t="shared" si="7"/>
+        <v>4.8414611816406253E-9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1024</v>
       </c>
@@ -4247,8 +4286,12 @@
         <f t="shared" si="6"/>
         <v>5.9866308593749999E-6</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73" s="1">
+        <f t="shared" si="7"/>
+        <v>5.8463191986083984E-9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2048</v>
       </c>
@@ -4259,8 +4302,12 @@
         <f t="shared" si="6"/>
         <v>1.30919921875E-5</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" s="1">
+        <f t="shared" si="7"/>
+        <v>6.3925743103027344E-9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4096</v>
       </c>
@@ -4271,8 +4318,12 @@
         <f t="shared" si="6"/>
         <v>3.368212890625E-5</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="1">
+        <f t="shared" si="7"/>
+        <v>8.2231760025024415E-9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>8192</v>
       </c>
@@ -4283,8 +4334,12 @@
         <f t="shared" si="6"/>
         <v>7.2394775390624997E-5</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" s="1">
+        <f t="shared" si="7"/>
+        <v>8.8372528553009029E-9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>16384</v>
       </c>
@@ -4295,13 +4350,17 @@
         <f t="shared" si="6"/>
         <v>1.5076538085937499E-4</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" s="1">
+        <f t="shared" si="7"/>
+        <v>9.2019885778427116E-9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -4311,8 +4370,11 @@
       <c r="C79" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2</v>
       </c>
@@ -4320,11 +4382,15 @@
         <v>3.7857799999999999E-7</v>
       </c>
       <c r="C80" s="1">
-        <f t="shared" ref="C80:C98" si="7">B80/A80</f>
+        <f t="shared" ref="C80:C98" si="8">B80/A80</f>
         <v>1.89289E-7</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" s="1">
+        <f t="shared" ref="D80:D98" si="9">C80/LOG(A80,2)</f>
+        <v>1.89289E-7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -4332,11 +4398,15 @@
         <v>6.1772499999999998E-7</v>
       </c>
       <c r="C81" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5443125E-7</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" s="1">
+        <f t="shared" si="9"/>
+        <v>7.7215624999999998E-8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>8</v>
       </c>
@@ -4344,11 +4414,15 @@
         <v>1.20864E-6</v>
       </c>
       <c r="C82" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5108E-7</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" s="1">
+        <f t="shared" si="9"/>
+        <v>5.0360000000000002E-8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>16</v>
       </c>
@@ -4356,11 +4430,15 @@
         <v>2.5235099999999999E-6</v>
       </c>
       <c r="C83" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5771937499999999E-7</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" s="1">
+        <f t="shared" si="9"/>
+        <v>3.9429843749999999E-8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>32</v>
       </c>
@@ -4368,11 +4446,15 @@
         <v>5.1906699999999997E-6</v>
       </c>
       <c r="C84" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6220843749999999E-7</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" s="1">
+        <f t="shared" si="9"/>
+        <v>3.2441687499999998E-8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>64</v>
       </c>
@@ -4380,11 +4462,15 @@
         <v>1.0754099999999999E-5</v>
       </c>
       <c r="C85" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6803281249999999E-7</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" s="1">
+        <f t="shared" si="9"/>
+        <v>2.8005468749999998E-8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>128</v>
       </c>
@@ -4392,11 +4478,15 @@
         <v>2.2574599999999999E-5</v>
       </c>
       <c r="C86" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.7636406249999999E-7</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" s="1">
+        <f t="shared" si="9"/>
+        <v>2.519486607142857E-8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>256</v>
       </c>
@@ -4404,11 +4494,15 @@
         <v>5.0451899999999997E-5</v>
       </c>
       <c r="C87" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.9707773437499999E-7</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" s="1">
+        <f t="shared" si="9"/>
+        <v>2.4634716796874999E-8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>512</v>
       </c>
@@ -4416,11 +4510,15 @@
         <v>1.04994E-4</v>
       </c>
       <c r="C88" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.0506640625000001E-7</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" s="1">
+        <f t="shared" si="9"/>
+        <v>2.278515625E-8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1024</v>
       </c>
@@ -4428,11 +4526,15 @@
         <v>2.29213E-4</v>
       </c>
       <c r="C89" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.238408203125E-7</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="1">
+        <f t="shared" si="9"/>
+        <v>2.238408203125E-8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2048</v>
       </c>
@@ -4440,11 +4542,15 @@
         <v>5.1689499999999996E-4</v>
       </c>
       <c r="C90" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.5239013671874998E-7</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" s="1">
+        <f t="shared" si="9"/>
+        <v>2.2944557883522725E-8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4096</v>
       </c>
@@ -4452,11 +4558,15 @@
         <v>1.15182E-3</v>
       </c>
       <c r="C91" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.812060546875E-7</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91" s="1">
+        <f t="shared" si="9"/>
+        <v>2.3433837890624999E-8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>8192</v>
       </c>
@@ -4464,11 +4574,15 @@
         <v>2.55033E-3</v>
       </c>
       <c r="C92" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.1131958007812499E-7</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" s="1">
+        <f t="shared" si="9"/>
+        <v>2.3947660006009614E-8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>16384</v>
       </c>
@@ -4476,11 +4590,15 @@
         <v>5.7246199999999997E-3</v>
       </c>
       <c r="C93" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.4940307617187498E-7</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" s="1">
+        <f t="shared" si="9"/>
+        <v>2.4957362583705355E-8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>32768</v>
       </c>
@@ -4488,11 +4606,15 @@
         <v>1.38245E-2</v>
       </c>
       <c r="C94" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.218902587890625E-7</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" s="1">
+        <f t="shared" si="9"/>
+        <v>2.8126017252604166E-8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>65536</v>
       </c>
@@ -4500,11 +4622,15 @@
         <v>3.2553699999999998E-2</v>
       </c>
       <c r="C95" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.9673004150390622E-7</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" s="1">
+        <f t="shared" si="9"/>
+        <v>3.1045627593994139E-8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>131072</v>
       </c>
@@ -4512,11 +4638,15 @@
         <v>8.4348500000000007E-2</v>
       </c>
       <c r="C96" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.4352798461914068E-7</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96" s="1">
+        <f t="shared" si="9"/>
+        <v>3.7854587330537688E-8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>262144</v>
       </c>
@@ -4524,11 +4654,15 @@
         <v>0.19187100000000001</v>
       </c>
       <c r="C97" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.3192977905273443E-7</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" s="1">
+        <f t="shared" si="9"/>
+        <v>4.066276550292969E-8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>524288</v>
       </c>
@@ -4536,16 +4670,20 @@
         <v>0.41272900000000001</v>
       </c>
       <c r="C98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.8721809387207034E-7</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98" s="1">
+        <f t="shared" si="9"/>
+        <v>4.1432531256424756E-8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -4555,8 +4693,11 @@
       <c r="C100" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2</v>
       </c>
@@ -4564,11 +4705,15 @@
         <v>4.1482200000000001E-7</v>
       </c>
       <c r="C101" s="1">
-        <f t="shared" ref="C101:C119" si="8">B101/A101</f>
+        <f t="shared" ref="C101:C119" si="10">B101/A101</f>
         <v>2.07411E-7</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" s="1">
+        <f t="shared" ref="D101:D119" si="11">C101/LOG(A101,2)</f>
+        <v>2.07411E-7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>4</v>
       </c>
@@ -4576,11 +4721,15 @@
         <v>7.5242599999999996E-7</v>
       </c>
       <c r="C102" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.8810649999999999E-7</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" s="1">
+        <f t="shared" si="11"/>
+        <v>9.4053249999999996E-8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>8</v>
       </c>
@@ -4588,11 +4737,15 @@
         <v>1.5342799999999999E-6</v>
       </c>
       <c r="C103" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9178499999999999E-7</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" s="1">
+        <f t="shared" si="11"/>
+        <v>6.3928333333333331E-8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>16</v>
       </c>
@@ -4600,11 +4753,15 @@
         <v>3.1552299999999999E-6</v>
       </c>
       <c r="C104" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9720187499999999E-7</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" s="1">
+        <f t="shared" si="11"/>
+        <v>4.9300468749999998E-8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>32</v>
       </c>
@@ -4612,11 +4769,15 @@
         <v>6.4649999999999999E-6</v>
       </c>
       <c r="C105" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.0203125E-7</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105" s="1">
+        <f t="shared" si="11"/>
+        <v>4.0406249999999998E-8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>64</v>
       </c>
@@ -4624,11 +4785,15 @@
         <v>1.28251E-5</v>
       </c>
       <c r="C106" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.003921875E-7</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" s="1">
+        <f t="shared" si="11"/>
+        <v>3.3398697916666665E-8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>128</v>
       </c>
@@ -4636,11 +4801,15 @@
         <v>2.5710900000000001E-5</v>
       </c>
       <c r="C107" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.0086640625000001E-7</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" s="1">
+        <f t="shared" si="11"/>
+        <v>2.8695200892857146E-8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>256</v>
       </c>
@@ -4648,11 +4817,15 @@
         <v>5.6993200000000002E-5</v>
       </c>
       <c r="C108" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.2262968750000001E-7</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" s="1">
+        <f t="shared" si="11"/>
+        <v>2.7828710937500001E-8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>512</v>
       </c>
@@ -4660,11 +4833,15 @@
         <v>1.2667900000000001E-4</v>
       </c>
       <c r="C109" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.4741992187500002E-7</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109" s="1">
+        <f t="shared" si="11"/>
+        <v>2.749110243055556E-8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1024</v>
       </c>
@@ -4672,11 +4849,15 @@
         <v>4.01748E-4</v>
       </c>
       <c r="C110" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.9233203125E-7</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110" s="1">
+        <f t="shared" si="11"/>
+        <v>3.9233203125E-8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2048</v>
       </c>
@@ -4684,11 +4865,15 @@
         <v>7.5248600000000002E-4</v>
       </c>
       <c r="C111" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6742480468750001E-7</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111" s="1">
+        <f t="shared" si="11"/>
+        <v>3.3402254971590908E-8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>4096</v>
       </c>
@@ -4696,11 +4881,15 @@
         <v>1.81302E-3</v>
       </c>
       <c r="C112" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.4263183593750001E-7</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112" s="1">
+        <f t="shared" si="11"/>
+        <v>3.6885986328124999E-8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>8192</v>
       </c>
@@ -4708,11 +4897,15 @@
         <v>4.1349500000000001E-3</v>
       </c>
       <c r="C113" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.0475463867187501E-7</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" s="1">
+        <f t="shared" si="11"/>
+        <v>3.8827279897836541E-8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>16384</v>
       </c>
@@ -4720,11 +4913,15 @@
         <v>9.3053100000000007E-3</v>
       </c>
       <c r="C114" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.6795104980468754E-7</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114" s="1">
+        <f t="shared" si="11"/>
+        <v>4.0567932128906253E-8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>32768</v>
       </c>
@@ -4732,11 +4929,15 @@
         <v>2.2083599999999998E-2</v>
       </c>
       <c r="C115" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.7393798828124995E-7</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115" s="1">
+        <f t="shared" si="11"/>
+        <v>4.4929199218749996E-8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>65536</v>
       </c>
@@ -4744,11 +4945,15 @@
         <v>5.4406999999999997E-2</v>
       </c>
       <c r="C116" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8.3018493652343745E-7</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116" s="1">
+        <f t="shared" si="11"/>
+        <v>5.1886558532714841E-8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>131072</v>
       </c>
@@ -4756,11 +4961,15 @@
         <v>0.14934800000000001</v>
       </c>
       <c r="C117" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.1394348144531251E-6</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117" s="1">
+        <f t="shared" si="11"/>
+        <v>6.702557732077206E-8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>262144</v>
       </c>
@@ -4768,11 +4977,15 @@
         <v>0.37943100000000002</v>
       </c>
       <c r="C118" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.4474143981933594E-6</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118" s="1">
+        <f t="shared" si="11"/>
+        <v>8.0411911010742191E-8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>524288</v>
       </c>
@@ -4780,8 +4993,12 @@
         <v>0.90140799999999999</v>
       </c>
       <c r="C119" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.71929931640625E-6</v>
+      </c>
+      <c r="D119" s="1">
+        <f t="shared" si="11"/>
+        <v>9.0489437705592098E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Graphs into jpegs
</commit_message>
<xml_diff>
--- a/report/timing.xlsx
+++ b/report/timing.xlsx
@@ -31,7 +31,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -639,11 +638,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412350152"/>
-        <c:axId val="412342704"/>
+        <c:axId val="129046392"/>
+        <c:axId val="129051096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412350152"/>
+        <c:axId val="129046392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,12 +754,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412342704"/>
+        <c:crossAx val="129051096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412342704"/>
+        <c:axId val="129051096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412350152"/>
+        <c:crossAx val="129046392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -968,7 +967,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -981,19 +980,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Random Height Big O Constant</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>AVL Trees </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1011,7 +1010,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1213,11 +1212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="472370704"/>
-        <c:axId val="472367176"/>
+        <c:axId val="359084712"/>
+        <c:axId val="359082752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="472370704"/>
+        <c:axId val="359084712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,7 +1243,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1257,7 +1256,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input Size</a:t>
                 </a:r>
               </a:p>
@@ -1277,7 +1276,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1315,7 +1314,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1330,12 +1329,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472367176"/>
+        <c:crossAx val="359082752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472367176"/>
+        <c:axId val="359082752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1361,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1375,7 +1374,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Big O Constant</a:t>
                 </a:r>
               </a:p>
@@ -1395,7 +1394,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1433,7 +1432,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1448,7 +1447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472370704"/>
+        <c:crossAx val="359084712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1513,7 +1512,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1526,20 +1525,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Linear </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Height Time per Insertion</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Binary Search Trees</a:t>
             </a:r>
           </a:p>
@@ -1559,7 +1558,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1731,11 +1730,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="472441160"/>
-        <c:axId val="472441552"/>
+        <c:axId val="359083536"/>
+        <c:axId val="359080008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="472441160"/>
+        <c:axId val="359083536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1761,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1775,14 +1774,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1800,7 +1799,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1838,7 +1837,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1853,12 +1852,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472441552"/>
+        <c:crossAx val="359080008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472441552"/>
+        <c:axId val="359080008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,7 +1884,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1898,7 +1897,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time per Insertion (sec)</a:t>
                 </a:r>
               </a:p>
@@ -1918,7 +1917,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1956,7 +1955,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1971,7 +1970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472441160"/>
+        <c:crossAx val="359083536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2036,7 +2035,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2049,19 +2048,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Linear Height Big O Constant</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Binary Search Trees </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2079,7 +2078,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2251,11 +2250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="463202912"/>
-        <c:axId val="463204872"/>
+        <c:axId val="359086672"/>
+        <c:axId val="359080792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="463202912"/>
+        <c:axId val="359086672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2282,7 +2281,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2295,7 +2294,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input Size</a:t>
                 </a:r>
               </a:p>
@@ -2315,7 +2314,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2353,7 +2352,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2368,12 +2367,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463204872"/>
+        <c:crossAx val="359080792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="463204872"/>
+        <c:axId val="359080792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2399,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2413,7 +2412,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Big O Constant</a:t>
                 </a:r>
               </a:p>
@@ -2433,7 +2432,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2471,7 +2470,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2486,7 +2485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463202912"/>
+        <c:crossAx val="359086672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2551,7 +2550,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2564,20 +2563,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Logarithmic </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Height Time per Insertion</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Binary Search Trees</a:t>
             </a:r>
           </a:p>
@@ -2597,7 +2596,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2799,11 +2798,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="472984944"/>
-        <c:axId val="472982592"/>
+        <c:axId val="359085104"/>
+        <c:axId val="359081968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="472984944"/>
+        <c:axId val="359085104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2830,7 +2829,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2843,14 +2842,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2868,7 +2867,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2906,7 +2905,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2921,12 +2920,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472982592"/>
+        <c:crossAx val="359081968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472982592"/>
+        <c:axId val="359081968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2953,7 +2952,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2966,7 +2965,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time per Insertion (sec)</a:t>
                 </a:r>
               </a:p>
@@ -2986,7 +2985,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3024,7 +3023,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3039,7 +3038,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472984944"/>
+        <c:crossAx val="359085104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3104,7 +3103,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3117,19 +3116,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Logarithmic Height Big O Constant</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Binary Search Trees </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3147,7 +3146,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3349,11 +3348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="472439592"/>
-        <c:axId val="472439984"/>
+        <c:axId val="359084320"/>
+        <c:axId val="359081576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="472439592"/>
+        <c:axId val="359084320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3380,7 +3379,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3393,7 +3392,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input Size</a:t>
                 </a:r>
               </a:p>
@@ -3413,7 +3412,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3451,7 +3450,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3466,12 +3465,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472439984"/>
+        <c:crossAx val="359081576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472439984"/>
+        <c:axId val="359081576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3498,7 +3497,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3511,7 +3510,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Big O Constant</a:t>
                 </a:r>
               </a:p>
@@ -3531,7 +3530,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3569,7 +3568,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3584,7 +3583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472439592"/>
+        <c:crossAx val="359084320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3649,7 +3648,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3662,24 +3661,24 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Random</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Height Time per Insertion</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Binary Search Trees</a:t>
             </a:r>
           </a:p>
@@ -3699,7 +3698,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3901,13 +3900,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="407650504"/>
-        <c:axId val="407653248"/>
+        <c:axId val="359085888"/>
+        <c:axId val="359086280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="407650504"/>
+        <c:axId val="359085888"/>
         <c:scaling>
-          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3933,7 +3931,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3946,14 +3944,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3971,7 +3969,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4009,7 +4007,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4024,12 +4022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407653248"/>
+        <c:crossAx val="359086280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="407653248"/>
+        <c:axId val="359086280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4056,7 +4054,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4069,7 +4067,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time per Insertion (sec)</a:t>
                 </a:r>
               </a:p>
@@ -4089,7 +4087,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4127,7 +4125,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4142,7 +4140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407650504"/>
+        <c:crossAx val="359085888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4207,7 +4205,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4220,19 +4218,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Random Height Big O Constant</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Binary Search Trees </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4250,7 +4248,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4452,11 +4450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="406108720"/>
-        <c:axId val="406105976"/>
+        <c:axId val="359087456"/>
+        <c:axId val="129460552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="406108720"/>
+        <c:axId val="359087456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4483,7 +4481,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4496,7 +4494,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input Size</a:t>
                 </a:r>
               </a:p>
@@ -4516,7 +4514,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4554,7 +4552,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4569,12 +4567,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406105976"/>
+        <c:crossAx val="129460552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="406105976"/>
+        <c:axId val="129460552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4601,7 +4599,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4614,7 +4612,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Big O Constant</a:t>
                 </a:r>
               </a:p>
@@ -4634,7 +4632,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4672,7 +4670,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4687,7 +4685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406108720"/>
+        <c:crossAx val="359087456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4752,7 +4750,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4765,23 +4763,23 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Comparison of Time</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t> per Addition</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>AVL Trees</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4798,7 +4796,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5230,13 +5228,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412348584"/>
-        <c:axId val="412351328"/>
+        <c:axId val="129053056"/>
+        <c:axId val="129053448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412348584"/>
+        <c:axId val="129053056"/>
         <c:scaling>
-          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5262,7 +5259,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5275,7 +5272,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Size</a:t>
                 </a:r>
               </a:p>
@@ -5294,7 +5291,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5332,7 +5329,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5347,12 +5344,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412351328"/>
+        <c:crossAx val="129053448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412351328"/>
+        <c:axId val="129053448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5379,7 +5376,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5392,7 +5389,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time  per Addition(sec)</a:t>
                 </a:r>
               </a:p>
@@ -5411,7 +5408,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5449,7 +5446,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5464,7 +5461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412348584"/>
+        <c:crossAx val="129053056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5560,7 +5557,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5573,19 +5570,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Comparison of Times </a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Binary Search Trees</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5602,7 +5599,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6034,11 +6031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412351720"/>
-        <c:axId val="412352504"/>
+        <c:axId val="358476616"/>
+        <c:axId val="358477792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412351720"/>
+        <c:axId val="358476616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6065,7 +6062,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6078,7 +6075,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Size</a:t>
                 </a:r>
               </a:p>
@@ -6097,7 +6094,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6135,7 +6132,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6150,12 +6147,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412352504"/>
+        <c:crossAx val="358477792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412352504"/>
+        <c:axId val="358477792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6182,7 +6179,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6195,7 +6192,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time (sec)</a:t>
                 </a:r>
               </a:p>
@@ -6214,7 +6211,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6252,7 +6249,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6267,7 +6264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412351720"/>
+        <c:crossAx val="358476616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6363,7 +6360,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6376,23 +6373,23 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Comparison of Time</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t> per Addition</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>AVL Trees</a:t>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t>Binary Search Trees</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6409,7 +6406,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6841,11 +6838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412353288"/>
-        <c:axId val="412350544"/>
+        <c:axId val="358478968"/>
+        <c:axId val="358482888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412353288"/>
+        <c:axId val="358478968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6872,7 +6869,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6885,7 +6882,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Size</a:t>
                 </a:r>
               </a:p>
@@ -6904,7 +6901,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6942,7 +6939,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6957,12 +6954,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412350544"/>
+        <c:crossAx val="358482888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412350544"/>
+        <c:axId val="358482888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6989,7 +6986,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -7002,7 +6999,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time  per Addition(sec)</a:t>
                 </a:r>
               </a:p>
@@ -7021,7 +7018,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -7059,7 +7056,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7074,7 +7071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412353288"/>
+        <c:crossAx val="358478968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7170,7 +7167,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7183,22 +7180,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Linear Height Time per Insertion</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>AVL Trees</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7212,7 +7208,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -7384,11 +7380,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="412353680"/>
-        <c:axId val="141768784"/>
+        <c:axId val="358481712"/>
+        <c:axId val="358479360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="412353680"/>
+        <c:axId val="358481712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7415,7 +7411,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -7428,18 +7424,17 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7453,7 +7448,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -7491,7 +7486,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7506,12 +7501,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141768784"/>
+        <c:crossAx val="358479360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141768784"/>
+        <c:axId val="358479360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7538,7 +7533,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -7551,13 +7546,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time per Insertion (sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7571,7 +7565,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -7609,7 +7603,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7624,7 +7618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412353680"/>
+        <c:crossAx val="358481712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7689,7 +7683,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7702,19 +7696,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Linear Height Big O Constant</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>AVL Trees </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -7732,7 +7725,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -7792,6 +7785,62 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$16</c:f>
@@ -7904,11 +7953,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141773488"/>
-        <c:axId val="141775056"/>
+        <c:axId val="358479752"/>
+        <c:axId val="358482104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141773488"/>
+        <c:axId val="358479752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7935,7 +7984,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -7948,7 +7997,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input Size</a:t>
                 </a:r>
               </a:p>
@@ -7968,7 +8017,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8006,7 +8055,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8021,12 +8070,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141775056"/>
+        <c:crossAx val="358482104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141775056"/>
+        <c:axId val="358482104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8053,7 +8102,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8066,7 +8115,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Big O Constant</a:t>
                 </a:r>
               </a:p>
@@ -8086,7 +8135,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8124,7 +8173,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8139,7 +8188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141773488"/>
+        <c:crossAx val="358479752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8204,7 +8253,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8217,24 +8266,24 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Logarithmic</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Height Time per Insertion</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>AVL Trees</a:t>
             </a:r>
           </a:p>
@@ -8254,7 +8303,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -8468,11 +8517,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="410562256"/>
-        <c:axId val="410563824"/>
+        <c:axId val="358478576"/>
+        <c:axId val="358482496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="410562256"/>
+        <c:axId val="358478576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8499,7 +8548,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8512,14 +8561,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -8537,7 +8586,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8575,7 +8624,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8590,12 +8639,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410563824"/>
+        <c:crossAx val="358482496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="410563824"/>
+        <c:axId val="358482496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8622,7 +8671,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8635,7 +8684,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time per Insertion (sec)</a:t>
                 </a:r>
               </a:p>
@@ -8655,7 +8704,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8693,7 +8742,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8708,7 +8757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410562256"/>
+        <c:crossAx val="358478576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8773,7 +8822,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8786,19 +8835,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Logithmic Height Big O Constant</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>AVL Trees </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -8816,7 +8865,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -9030,11 +9079,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="472353512"/>
-        <c:axId val="472352336"/>
+        <c:axId val="358480144"/>
+        <c:axId val="358483672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="472353512"/>
+        <c:axId val="358480144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9061,7 +9110,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9074,7 +9123,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input Size</a:t>
                 </a:r>
               </a:p>
@@ -9094,7 +9143,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9132,7 +9181,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9147,12 +9196,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472352336"/>
+        <c:crossAx val="358483672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="472352336"/>
+        <c:axId val="358483672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9179,7 +9228,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9192,7 +9241,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Big O Constant</a:t>
                 </a:r>
               </a:p>
@@ -9212,7 +9261,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9250,7 +9299,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9265,7 +9314,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472353512"/>
+        <c:crossAx val="358480144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9330,7 +9379,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9343,20 +9392,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
               <a:t>Random </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>Height Time per Insertion</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800"/>
               <a:t>AVL Trees</a:t>
             </a:r>
           </a:p>
@@ -9376,7 +9425,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -9578,11 +9627,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="462877128"/>
-        <c:axId val="462877912"/>
+        <c:axId val="358477008"/>
+        <c:axId val="358481320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="462877128"/>
+        <c:axId val="358477008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9609,7 +9658,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9622,14 +9671,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Input</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
                   <a:t> Size</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -9647,7 +9696,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9685,7 +9734,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9700,12 +9749,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="462877912"/>
+        <c:crossAx val="358481320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="462877912"/>
+        <c:axId val="358481320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9732,7 +9781,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9745,7 +9794,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Time per Insertion (sec)</a:t>
                 </a:r>
               </a:p>
@@ -9765,7 +9814,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9803,7 +9852,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9818,7 +9867,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="462877128"/>
+        <c:crossAx val="358477008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
Finished Report (may need proofreading)
</commit_message>
<xml_diff>
--- a/report/timing.xlsx
+++ b/report/timing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4092" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4092" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison (AVL Tree)" sheetId="2" r:id="rId1"/>
@@ -638,11 +638,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="129046392"/>
-        <c:axId val="129051096"/>
+        <c:axId val="129086056"/>
+        <c:axId val="129087624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="129046392"/>
+        <c:axId val="129086056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,12 +754,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129051096"/>
+        <c:crossAx val="129087624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129051096"/>
+        <c:axId val="129087624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,7 +871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129046392"/>
+        <c:crossAx val="129086056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1212,11 +1212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359084712"/>
-        <c:axId val="359082752"/>
+        <c:axId val="360872936"/>
+        <c:axId val="360876072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359084712"/>
+        <c:axId val="360872936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1329,12 +1329,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359082752"/>
+        <c:crossAx val="360876072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359082752"/>
+        <c:axId val="360876072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359084712"/>
+        <c:crossAx val="360872936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1730,11 +1730,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359083536"/>
-        <c:axId val="359080008"/>
+        <c:axId val="360873720"/>
+        <c:axId val="360874112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359083536"/>
+        <c:axId val="360873720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,12 +1852,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359080008"/>
+        <c:crossAx val="360874112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359080008"/>
+        <c:axId val="360874112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,7 +1970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359083536"/>
+        <c:crossAx val="360873720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2250,11 +2250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359086672"/>
-        <c:axId val="359080792"/>
+        <c:axId val="360877640"/>
+        <c:axId val="360874504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359086672"/>
+        <c:axId val="360877640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,12 +2367,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359080792"/>
+        <c:crossAx val="360874504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359080792"/>
+        <c:axId val="360874504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,7 +2485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359086672"/>
+        <c:crossAx val="360877640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2798,11 +2798,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359085104"/>
-        <c:axId val="359081968"/>
+        <c:axId val="360878032"/>
+        <c:axId val="360878424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359085104"/>
+        <c:axId val="360878032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2920,12 +2920,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359081968"/>
+        <c:crossAx val="360878424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359081968"/>
+        <c:axId val="360878424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3038,7 +3038,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359085104"/>
+        <c:crossAx val="360878032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3348,11 +3348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359084320"/>
-        <c:axId val="359081576"/>
+        <c:axId val="360655888"/>
+        <c:axId val="360654320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359084320"/>
+        <c:axId val="360655888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3465,12 +3465,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359081576"/>
+        <c:crossAx val="360654320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359081576"/>
+        <c:axId val="360654320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3583,7 +3583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359084320"/>
+        <c:crossAx val="360655888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3900,11 +3900,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359085888"/>
-        <c:axId val="359086280"/>
+        <c:axId val="360654712"/>
+        <c:axId val="360655104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359085888"/>
+        <c:axId val="360654712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4022,12 +4022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359086280"/>
+        <c:crossAx val="360655104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359086280"/>
+        <c:axId val="360655104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4140,7 +4140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359085888"/>
+        <c:crossAx val="360654712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4450,11 +4450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359087456"/>
-        <c:axId val="129460552"/>
+        <c:axId val="360655496"/>
+        <c:axId val="360656280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359087456"/>
+        <c:axId val="360655496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4567,12 +4567,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129460552"/>
+        <c:crossAx val="360656280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129460552"/>
+        <c:axId val="360656280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4685,7 +4685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359087456"/>
+        <c:crossAx val="360655496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5228,11 +5228,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="129053056"/>
-        <c:axId val="129053448"/>
+        <c:axId val="129091152"/>
+        <c:axId val="129088800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="129053056"/>
+        <c:axId val="129091152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5344,12 +5344,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129053448"/>
+        <c:crossAx val="129088800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129053448"/>
+        <c:axId val="129088800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5461,7 +5461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129053056"/>
+        <c:crossAx val="129091152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6031,11 +6031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358476616"/>
-        <c:axId val="358477792"/>
+        <c:axId val="129089584"/>
+        <c:axId val="129089976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358476616"/>
+        <c:axId val="129089584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6147,12 +6147,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358477792"/>
+        <c:crossAx val="129089976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358477792"/>
+        <c:axId val="129089976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6264,7 +6264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358476616"/>
+        <c:crossAx val="129089584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6838,11 +6838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358478968"/>
-        <c:axId val="358482888"/>
+        <c:axId val="359784992"/>
+        <c:axId val="359786560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358478968"/>
+        <c:axId val="359784992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6954,12 +6954,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358482888"/>
+        <c:crossAx val="359786560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358482888"/>
+        <c:axId val="359786560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7071,7 +7071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358478968"/>
+        <c:crossAx val="359784992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7380,11 +7380,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358481712"/>
-        <c:axId val="358479360"/>
+        <c:axId val="359786168"/>
+        <c:axId val="359787344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358481712"/>
+        <c:axId val="359786168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7501,12 +7501,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358479360"/>
+        <c:crossAx val="359787344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358479360"/>
+        <c:axId val="359787344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7618,7 +7618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358481712"/>
+        <c:crossAx val="359786168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7711,7 +7711,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7953,11 +7952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358479752"/>
-        <c:axId val="358482104"/>
+        <c:axId val="359788128"/>
+        <c:axId val="359785384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358479752"/>
+        <c:axId val="359788128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8003,7 +8002,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8070,12 +8068,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358482104"/>
+        <c:crossAx val="359785384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358482104"/>
+        <c:axId val="359785384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8121,7 +8119,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8188,7 +8185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358479752"/>
+        <c:crossAx val="359788128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8289,7 +8286,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8517,11 +8513,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358478576"/>
-        <c:axId val="358482496"/>
+        <c:axId val="360876856"/>
+        <c:axId val="360871760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358478576"/>
+        <c:axId val="360876856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8572,7 +8568,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8639,12 +8634,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358482496"/>
+        <c:crossAx val="360871760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358482496"/>
+        <c:axId val="360871760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8690,7 +8685,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8757,7 +8751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358478576"/>
+        <c:crossAx val="360876856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9079,11 +9073,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358480144"/>
-        <c:axId val="358483672"/>
+        <c:axId val="360876464"/>
+        <c:axId val="360875680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358480144"/>
+        <c:axId val="360876464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9196,12 +9190,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358483672"/>
+        <c:crossAx val="360875680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358483672"/>
+        <c:axId val="360875680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9314,7 +9308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358480144"/>
+        <c:crossAx val="360876464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9627,11 +9621,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358477008"/>
-        <c:axId val="358481320"/>
+        <c:axId val="360871368"/>
+        <c:axId val="360877248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="358477008"/>
+        <c:axId val="360871368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9749,12 +9743,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358481320"/>
+        <c:crossAx val="360877248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358481320"/>
+        <c:axId val="360877248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9867,7 +9861,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358477008"/>
+        <c:crossAx val="360871368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18888,7 +18882,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19680,8 +19674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101:D119"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>